<commit_message>
feat: improve documentation for import process of samples and chemicals
</commit_message>
<xml_diff>
--- a/static/files/template_sample_import.xlsx
+++ b/static/files/template_sample_import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49172\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3372A5C4-1E3E-47FE-B3B7-C0324DB0BB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BDAF07-9F61-405D-92F9-6244CA5030DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="73">
   <si>
     <t>residue type</t>
   </si>
@@ -229,24 +229,6 @@
   </si>
   <si>
     <t>refractive index</t>
-  </si>
-  <si>
-    <t>shelf 1</t>
-  </si>
-  <si>
-    <t>shelf 3</t>
-  </si>
-  <si>
-    <t>shelf 4</t>
-  </si>
-  <si>
-    <t>shelf 5</t>
-  </si>
-  <si>
-    <t>shelf 6</t>
-  </si>
-  <si>
-    <t>shelf 2</t>
   </si>
   <si>
     <t>4,0 g/ml</t>
@@ -268,7 +250,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -299,11 +281,6 @@
       <name val="Calibri"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -343,21 +320,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Normal" xfId="1" xr:uid="{6D34E690-39F4-46A0-A6E9-56A02EA48096}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -441,7 +416,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -760,10 +735,10 @@
   <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="AC20" sqref="AC20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -788,7 +763,7 @@
     <col min="25" max="25" width="10.85546875" customWidth="1"/>
     <col min="26" max="26" width="9.5703125" customWidth="1"/>
     <col min="27" max="27" width="27.5703125" customWidth="1"/>
-    <col min="28" max="28" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.140625" customWidth="1"/>
     <col min="29" max="30" width="15" customWidth="1"/>
     <col min="31" max="31" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="16.85546875" bestFit="1" customWidth="1"/>
@@ -818,7 +793,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -845,7 +820,7 @@
         <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>15</v>
@@ -886,12 +861,8 @@
       <c r="AD1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AE1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF1" s="5" t="s">
-        <v>60</v>
-      </c>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
     </row>
     <row r="2" spans="1:32" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
@@ -907,7 +878,7 @@
         <v>27</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>28</v>
@@ -935,7 +906,7 @@
       </c>
       <c r="Q2" s="3"/>
       <c r="R2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>29</v>
@@ -963,12 +934,6 @@
       </c>
       <c r="AD2">
         <v>1.33</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1010,7 +975,7 @@
         <v>31</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="T3" s="3" t="s">
         <v>29</v>
@@ -1032,12 +997,6 @@
       </c>
       <c r="AD3">
         <v>1.34</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1100,9 +1059,6 @@
       <c r="AD4">
         <v>1.35</v>
       </c>
-      <c r="AE4" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -1164,9 +1120,6 @@
       <c r="AD5">
         <v>1.36</v>
       </c>
-      <c r="AE5" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
@@ -1225,9 +1178,6 @@
       <c r="AD6">
         <v>1.37</v>
       </c>
-      <c r="AE6" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="7" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -1288,9 +1238,6 @@
       </c>
       <c r="AD7">
         <v>1.38</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: improve documentation for import process of samples and chemicals (#403)
Co-authored-by: adambasha0 <readam@adbasha>
</commit_message>
<xml_diff>
--- a/static/files/template_sample_import.xlsx
+++ b/static/files/template_sample_import.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\49172\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3372A5C4-1E3E-47FE-B3B7-C0324DB0BB87}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85BDAF07-9F61-405D-92F9-6244CA5030DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="sample" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132" uniqueCount="73">
   <si>
     <t>residue type</t>
   </si>
@@ -229,24 +229,6 @@
   </si>
   <si>
     <t>refractive index</t>
-  </si>
-  <si>
-    <t>shelf 1</t>
-  </si>
-  <si>
-    <t>shelf 3</t>
-  </si>
-  <si>
-    <t>shelf 4</t>
-  </si>
-  <si>
-    <t>shelf 5</t>
-  </si>
-  <si>
-    <t>shelf 6</t>
-  </si>
-  <si>
-    <t>shelf 2</t>
   </si>
   <si>
     <t>4,0 g/ml</t>
@@ -268,7 +250,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -299,11 +281,6 @@
       <name val="Calibri"/>
       <family val="1"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="1"/>
     </font>
     <font>
       <sz val="12"/>
@@ -343,21 +320,19 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Normal" xfId="1" xr:uid="{6D34E690-39F4-46A0-A6E9-56A02EA48096}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -441,7 +416,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -760,10 +735,10 @@
   <dimension ref="A1:AF7"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="AC20" sqref="AC20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.140625" customWidth="1"/>
     <col min="2" max="2" width="12" customWidth="1"/>
@@ -788,7 +763,7 @@
     <col min="25" max="25" width="10.85546875" customWidth="1"/>
     <col min="26" max="26" width="9.5703125" customWidth="1"/>
     <col min="27" max="27" width="27.5703125" customWidth="1"/>
-    <col min="28" max="28" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.140625" customWidth="1"/>
     <col min="29" max="30" width="15" customWidth="1"/>
     <col min="31" max="31" width="18.7109375" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="16.85546875" bestFit="1" customWidth="1"/>
@@ -818,7 +793,7 @@
         <v>6</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>7</v>
@@ -845,7 +820,7 @@
         <v>14</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>15</v>
@@ -886,12 +861,8 @@
       <c r="AD1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AE1" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="AF1" s="5" t="s">
-        <v>60</v>
-      </c>
+      <c r="AE1" s="5"/>
+      <c r="AF1" s="5"/>
     </row>
     <row r="2" spans="1:32" ht="15" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
@@ -907,7 +878,7 @@
         <v>27</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="I2" s="3" t="s">
         <v>28</v>
@@ -935,7 +906,7 @@
       </c>
       <c r="Q2" s="3"/>
       <c r="R2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="T2" s="3" t="s">
         <v>29</v>
@@ -963,12 +934,6 @@
       </c>
       <c r="AD2">
         <v>1.33</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1010,7 +975,7 @@
         <v>31</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="T3" s="3" t="s">
         <v>29</v>
@@ -1032,12 +997,6 @@
       </c>
       <c r="AD3">
         <v>1.34</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>73</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -1100,9 +1059,6 @@
       <c r="AD4">
         <v>1.35</v>
       </c>
-      <c r="AE4" t="s">
-        <v>69</v>
-      </c>
     </row>
     <row r="5" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -1164,9 +1120,6 @@
       <c r="AD5">
         <v>1.36</v>
       </c>
-      <c r="AE5" t="s">
-        <v>70</v>
-      </c>
     </row>
     <row r="6" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="3" t="s">
@@ -1225,9 +1178,6 @@
       <c r="AD6">
         <v>1.37</v>
       </c>
-      <c r="AE6" t="s">
-        <v>71</v>
-      </c>
     </row>
     <row r="7" spans="1:32" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="3" t="s">
@@ -1288,9 +1238,6 @@
       </c>
       <c r="AD7">
         <v>1.38</v>
-      </c>
-      <c r="AE7" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>